<commit_message>
edited mock data to avoid a bug.
</commit_message>
<xml_diff>
--- a/data/mock/feature_attrs.xlsx
+++ b/data/mock/feature_attrs.xlsx
@@ -416,7 +416,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -578,6 +578,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
@@ -592,6 +595,9 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
@@ -605,6 +611,9 @@
       </c>
       <c r="D10">
         <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>